<commit_message>
Added differences between matices in al elements
</commit_message>
<xml_diff>
--- a/1_data/chemical_analyses/icp_results.xlsx
+++ b/1_data/chemical_analyses/icp_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longchamp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iCAP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -686,18 +686,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -744,13 +738,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1041,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,6 +1121,12 @@
       <c r="D3" s="4">
         <v>1.27</v>
       </c>
+      <c r="E3" s="13">
+        <v>29042.388525547438</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.5349999999999999</v>
+      </c>
       <c r="G3" s="3">
         <v>2175.1734277372261</v>
       </c>
@@ -1165,6 +1165,12 @@
       <c r="D4" s="4">
         <v>0.81599999999999995</v>
       </c>
+      <c r="E4" s="13">
+        <v>25991.574761904762</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.8260000000000001</v>
+      </c>
       <c r="G4" s="3">
         <v>2351.3059444444448</v>
       </c>
@@ -1203,6 +1209,12 @@
       <c r="D5" s="4">
         <v>0.81879999999999997</v>
       </c>
+      <c r="E5" s="13">
+        <v>21738.74769230769</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.9390000000000001</v>
+      </c>
       <c r="G5" s="3">
         <v>2305.6247552447549</v>
       </c>
@@ -1241,6 +1253,12 @@
       <c r="D6" s="4">
         <v>0.69310000000000005</v>
       </c>
+      <c r="E6" s="13">
+        <v>26614.710867052025</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2.5609999999999999</v>
+      </c>
       <c r="G6" s="3">
         <v>2125.9678612716766</v>
       </c>
@@ -1279,6 +1297,12 @@
       <c r="D7" s="4">
         <v>0.78539999999999999</v>
       </c>
+      <c r="E7" s="13">
+        <v>16646.026248366015</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.4609999999999999</v>
+      </c>
       <c r="G7" s="3">
         <v>2675.0263093681915</v>
       </c>
@@ -1317,6 +1341,12 @@
       <c r="D8" s="4">
         <v>1.0289999999999999</v>
       </c>
+      <c r="E8" s="13">
+        <v>25994.506784140976</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.8891</v>
+      </c>
       <c r="G8" s="3">
         <v>2084.9056289769946</v>
       </c>
@@ -1355,6 +1385,12 @@
       <c r="D9" s="4">
         <v>0.35039999999999999</v>
       </c>
+      <c r="E9" s="13">
+        <v>15407.570795513377</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2.5259999999999998</v>
+      </c>
       <c r="G9" s="3">
         <v>2748.6162398619495</v>
       </c>
@@ -1393,6 +1429,12 @@
       <c r="D10" s="4">
         <v>0.80389999999999995</v>
       </c>
+      <c r="E10" s="13">
+        <v>20956.065207877462</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2.4689999999999999</v>
+      </c>
       <c r="G10" s="3">
         <v>2455.8356017505475</v>
       </c>
@@ -1431,6 +1473,12 @@
       <c r="D11" s="4">
         <v>0.89780000000000004</v>
       </c>
+      <c r="E11" s="13">
+        <v>20680.083672823217</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2.44</v>
+      </c>
       <c r="G11" s="3">
         <v>2286.819666490765</v>
       </c>
@@ -1469,6 +1517,12 @@
       <c r="D12" s="4">
         <v>0.70320000000000005</v>
       </c>
+      <c r="E12" s="13">
+        <v>24746.958977900551</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.1640000000000001</v>
+      </c>
       <c r="G12" s="3">
         <v>2129.0359571823196</v>
       </c>
@@ -1507,6 +1561,12 @@
       <c r="D13" s="4">
         <v>0.42370000000000002</v>
       </c>
+      <c r="E13" s="13">
+        <v>26298.962799377914</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3.2080000000000002</v>
+      </c>
       <c r="G13" s="3">
         <v>2346.1623592534988</v>
       </c>
@@ -1545,6 +1605,12 @@
       <c r="D14" s="4">
         <v>1.3</v>
       </c>
+      <c r="E14" s="13">
+        <v>21623.84818582299</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.194</v>
+      </c>
       <c r="G14" s="3">
         <v>2156.0354185022024</v>
       </c>
@@ -1583,6 +1649,12 @@
       <c r="D15" s="4">
         <v>3.206</v>
       </c>
+      <c r="E15" s="13">
+        <v>23848.382097421203</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1.8580000000000001</v>
+      </c>
       <c r="G15" s="3">
         <v>2318.4031060171919</v>
       </c>
@@ -1621,6 +1693,12 @@
       <c r="D16" s="4">
         <v>0.51659999999999995</v>
       </c>
+      <c r="E16" s="13">
+        <v>14771.01112479015</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.762</v>
+      </c>
       <c r="G16" s="3">
         <v>2482.3816116396192</v>
       </c>
@@ -1659,6 +1737,12 @@
       <c r="D17" s="4">
         <v>0.72829999999999995</v>
       </c>
+      <c r="E17" s="13">
+        <v>20652.35172046825</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1.0580000000000001</v>
+      </c>
       <c r="G17" s="3">
         <v>2130.4399255054982</v>
       </c>
@@ -1697,6 +1781,12 @@
       <c r="D18" s="4">
         <v>1.373</v>
       </c>
+      <c r="E18" s="13">
+        <v>27625.509765329298</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.31</v>
+      </c>
       <c r="G18" s="3">
         <v>2377.0160484481453</v>
       </c>
@@ -1735,6 +1825,12 @@
       <c r="D19" s="4">
         <v>0.90790000000000004</v>
       </c>
+      <c r="E19" s="13">
+        <v>29037.413296778606</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.6419999999999999</v>
+      </c>
       <c r="G19" s="3">
         <v>2340.4289239204932</v>
       </c>
@@ -1773,6 +1869,12 @@
       <c r="D20" s="4">
         <v>2.3579538653553707</v>
       </c>
+      <c r="E20" s="13">
+        <v>25737.49822900763</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3.3570000000000002</v>
+      </c>
       <c r="G20" s="3">
         <v>2033.2038727735369</v>
       </c>
@@ -1811,6 +1913,12 @@
       <c r="D21" s="4">
         <v>0.67510000000000003</v>
       </c>
+      <c r="E21" s="13">
+        <v>27048.311964549477</v>
+      </c>
+      <c r="F21" s="4">
+        <v>2.4</v>
+      </c>
       <c r="G21" s="3">
         <v>2087.6596750369276</v>
       </c>
@@ -1849,6 +1957,12 @@
       <c r="D22" s="4">
         <v>0.74129999999999996</v>
       </c>
+      <c r="E22" s="13">
+        <v>20276.124310776944</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.893</v>
+      </c>
       <c r="G22" s="3">
         <v>2171.4779030910609</v>
       </c>
@@ -1887,6 +2001,12 @@
       <c r="D23" s="4">
         <v>1.546</v>
       </c>
+      <c r="E23" s="13">
+        <v>23995.246979848867</v>
+      </c>
+      <c r="F23" s="4">
+        <v>3.645</v>
+      </c>
       <c r="G23" s="3">
         <v>2331.8196889168767</v>
       </c>
@@ -1925,6 +2045,12 @@
       <c r="D24" s="4">
         <v>1.0680000000000001</v>
       </c>
+      <c r="E24" s="13">
+        <v>30224.432368421054</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.42380000000000001</v>
+      </c>
       <c r="G24" s="3">
         <v>1838.9092105263157</v>
       </c>
@@ -1963,6 +2089,12 @@
       <c r="D25" s="4">
         <v>1.06</v>
       </c>
+      <c r="E25" s="13">
+        <v>22030.313820224721</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1.042</v>
+      </c>
       <c r="G25" s="3">
         <v>2168.3505009363298</v>
       </c>
@@ -2001,6 +2133,12 @@
       <c r="D26" s="4">
         <v>0.5141</v>
       </c>
+      <c r="E26" s="13">
+        <v>24592.225275142315</v>
+      </c>
+      <c r="F26" s="4">
+        <v>3.6459999999999999</v>
+      </c>
       <c r="G26" s="3">
         <v>2128.0777229601517</v>
       </c>
@@ -2039,6 +2177,12 @@
       <c r="D27" s="4">
         <v>1.583</v>
       </c>
+      <c r="E27" s="13">
+        <v>30119.794434447304</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2.6960000000000002</v>
+      </c>
       <c r="G27" s="3">
         <v>2215.0762660668383</v>
       </c>
@@ -2077,6 +2221,12 @@
       <c r="D28" s="4">
         <v>0.99250000000000005</v>
       </c>
+      <c r="E28" s="13">
+        <v>30818.000677637945</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.5609999999999999</v>
+      </c>
       <c r="G28" s="3">
         <v>2511.5363697967086</v>
       </c>
@@ -2115,6 +2265,12 @@
       <c r="D29" s="4">
         <v>1.042</v>
       </c>
+      <c r="E29" s="13">
+        <v>16268.652396373054</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2400000000000002</v>
+      </c>
       <c r="G29" s="3">
         <v>2676.9143393782379</v>
       </c>
@@ -2153,6 +2309,12 @@
       <c r="D30" s="4">
         <v>1.24</v>
       </c>
+      <c r="E30" s="13">
+        <v>16519.813745290132</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3.3540000000000001</v>
+      </c>
       <c r="G30" s="3">
         <v>2897.9361266013561</v>
       </c>
@@ -2191,6 +2353,12 @@
       <c r="D31" s="4">
         <v>0.8679</v>
       </c>
+      <c r="E31" s="13">
+        <v>23186.938601997146</v>
+      </c>
+      <c r="F31" s="4">
+        <v>3.16</v>
+      </c>
       <c r="G31" s="3">
         <v>2101.3662482168324</v>
       </c>
@@ -2229,6 +2397,12 @@
       <c r="D32" s="4">
         <v>0.84079999999999999</v>
       </c>
+      <c r="E32" s="13">
+        <v>27598.182505822075</v>
+      </c>
+      <c r="F32" s="4">
+        <v>3.4060000000000001</v>
+      </c>
       <c r="G32" s="3">
         <v>1862.6595621797858</v>
       </c>
@@ -2267,6 +2441,12 @@
       <c r="D33" s="4">
         <v>0.92918105280756036</v>
       </c>
+      <c r="E33" s="13">
+        <v>20914.359318885447</v>
+      </c>
+      <c r="F33" s="4">
+        <v>3.6280000000000001</v>
+      </c>
       <c r="G33" s="3">
         <v>2183.0505237358102</v>
       </c>
@@ -2305,6 +2485,12 @@
       <c r="D34" s="4">
         <v>0.89849999999999997</v>
       </c>
+      <c r="E34" s="13">
+        <v>28482.67693154034</v>
+      </c>
+      <c r="F34" s="4">
+        <v>2.867</v>
+      </c>
       <c r="G34" s="3">
         <v>1794.0476039119803</v>
       </c>
@@ -2343,6 +2529,12 @@
       <c r="D35" s="4">
         <v>0.58779999999999999</v>
       </c>
+      <c r="E35" s="13">
+        <v>14830.444664107486</v>
+      </c>
+      <c r="F35" s="4">
+        <v>4.077</v>
+      </c>
       <c r="G35" s="3">
         <v>2521.2714587332043</v>
       </c>
@@ -2381,6 +2573,12 @@
       <c r="D36" s="4">
         <v>0.84350000000000003</v>
       </c>
+      <c r="E36" s="13">
+        <v>21161.801863833898</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.1459999999999999</v>
+      </c>
       <c r="G36" s="3">
         <v>2142.5033220666346</v>
       </c>
@@ -2419,6 +2617,12 @@
       <c r="D37" s="4">
         <v>0.434</v>
       </c>
+      <c r="E37" s="13">
+        <v>29384.709010989012</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1.3497266236858787</v>
+      </c>
       <c r="G37" s="3">
         <v>2252.9315604395601</v>
       </c>
@@ -2457,6 +2661,12 @@
       <c r="D38" s="4">
         <v>0.80269999999999997</v>
       </c>
+      <c r="E38" s="13">
+        <v>31414.17316455696</v>
+      </c>
+      <c r="F38" s="4">
+        <v>2.069</v>
+      </c>
       <c r="G38" s="3">
         <v>2377.4276540084384</v>
       </c>
@@ -2495,6 +2705,12 @@
       <c r="D39" s="4">
         <v>0.54879999999999995</v>
       </c>
+      <c r="E39" s="13">
+        <v>28239.025327510913</v>
+      </c>
+      <c r="F39" s="4">
+        <v>2.9990000000000001</v>
+      </c>
       <c r="G39" s="3">
         <v>1948.8904803493447</v>
       </c>
@@ -2533,6 +2749,12 @@
       <c r="D40" s="4">
         <v>0.66659999999999997</v>
       </c>
+      <c r="E40" s="13">
+        <v>28293.831641791039</v>
+      </c>
+      <c r="F40" s="4">
+        <v>2.762</v>
+      </c>
       <c r="G40" s="3">
         <v>2021.5032039800997</v>
       </c>
@@ -2571,6 +2793,12 @@
       <c r="D41" s="4">
         <v>0.64749999999999996</v>
       </c>
+      <c r="E41" s="13">
+        <v>29396.271238813006</v>
+      </c>
+      <c r="F41" s="4">
+        <v>2.3530000000000002</v>
+      </c>
       <c r="G41" s="3">
         <v>2046.3635233160619</v>
       </c>
@@ -2609,6 +2837,12 @@
       <c r="D42" s="4">
         <v>0.71009999999999995</v>
       </c>
+      <c r="E42" s="13">
+        <v>29041.280397163118</v>
+      </c>
+      <c r="F42" s="4">
+        <v>2.8570000000000002</v>
+      </c>
       <c r="G42" s="3">
         <v>2015.6953286052012</v>
       </c>
@@ -2647,6 +2881,12 @@
       <c r="D43" s="4">
         <v>0.76485319760577919</v>
       </c>
+      <c r="E43" s="13">
+        <v>23280.812542843905</v>
+      </c>
+      <c r="F43" s="4">
+        <v>3.8290000000000002</v>
+      </c>
       <c r="G43" s="3">
         <v>2323.0922788327925</v>
       </c>
@@ -2685,6 +2925,12 @@
       <c r="D44" s="4">
         <v>2.9255555696585424E-2</v>
       </c>
+      <c r="E44" s="13">
+        <v>30255.815274863609</v>
+      </c>
+      <c r="F44" s="4">
+        <v>2.903</v>
+      </c>
       <c r="G44" s="3">
         <v>2116.1897629039026</v>
       </c>
@@ -2723,6 +2969,12 @@
       <c r="D45" s="4">
         <v>1.153</v>
       </c>
+      <c r="E45" s="13">
+        <v>27907.381876892021</v>
+      </c>
+      <c r="F45" s="4">
+        <v>2.6280000000000001</v>
+      </c>
       <c r="G45" s="3">
         <v>1873.2200605449041</v>
       </c>
@@ -2761,6 +3013,12 @@
       <c r="D46" s="4">
         <v>0.62909999999999999</v>
       </c>
+      <c r="E46" s="13">
+        <v>27744.874719101128</v>
+      </c>
+      <c r="F46" s="4">
+        <v>4.8609999999999998</v>
+      </c>
       <c r="G46" s="3">
         <v>2020.2066573033705</v>
       </c>
@@ -2799,6 +3057,12 @@
       <c r="D47" s="4">
         <v>1.2450000000000001</v>
       </c>
+      <c r="E47" s="13">
+        <v>30585.894554883314</v>
+      </c>
+      <c r="F47" s="4">
+        <v>3.5739999999999998</v>
+      </c>
       <c r="G47" s="3">
         <v>2139.922212618842</v>
       </c>
@@ -2837,6 +3101,12 @@
       <c r="D48" s="4">
         <v>0.91900000000000004</v>
       </c>
+      <c r="E48" s="13">
+        <v>27641.470560378846</v>
+      </c>
+      <c r="F48" s="4">
+        <v>4.3499999999999996</v>
+      </c>
       <c r="G48" s="3">
         <v>2304.839337016575</v>
       </c>
@@ -2875,6 +3145,12 @@
       <c r="D49" s="4">
         <v>1.19</v>
       </c>
+      <c r="E49" s="13">
+        <v>27375.359881188113</v>
+      </c>
+      <c r="F49" s="4">
+        <v>3.2309999999999999</v>
+      </c>
       <c r="G49" s="3">
         <v>2113.9529900990092</v>
       </c>
@@ -2913,6 +3189,12 @@
       <c r="D50" s="4">
         <v>0.59199999999999997</v>
       </c>
+      <c r="E50" s="13">
+        <v>26714.496875912409</v>
+      </c>
+      <c r="F50" s="4">
+        <v>2.0880000000000001</v>
+      </c>
       <c r="G50" s="3">
         <v>2032.0357664233575</v>
       </c>
@@ -2951,6 +3233,12 @@
       <c r="D51" s="4">
         <v>0.95860000000000001</v>
       </c>
+      <c r="E51" s="13">
+        <v>27683.027007434946</v>
+      </c>
+      <c r="F51" s="4">
+        <v>3.9870000000000001</v>
+      </c>
       <c r="G51" s="3">
         <v>1963.5161013011152</v>
       </c>
@@ -2989,6 +3277,12 @@
       <c r="D52" s="4">
         <v>0.96299999999999997</v>
       </c>
+      <c r="E52" s="13">
+        <v>28432.491896623589</v>
+      </c>
+      <c r="F52" s="4">
+        <v>2.6440000000000001</v>
+      </c>
       <c r="G52" s="3">
         <v>1744.8935139641515</v>
       </c>
@@ -3027,6 +3321,12 @@
       <c r="D53" s="4">
         <v>1.3710190899687043</v>
       </c>
+      <c r="E53" s="13">
+        <v>28696.79514035895</v>
+      </c>
+      <c r="F53" s="4">
+        <v>3.8340000000000001</v>
+      </c>
       <c r="G53" s="3">
         <v>1884.9293511274736</v>
       </c>
@@ -3065,6 +3365,12 @@
       <c r="D54" s="4">
         <v>0.3493</v>
       </c>
+      <c r="E54" s="13">
+        <v>32091.569441368902</v>
+      </c>
+      <c r="F54" s="4">
+        <v>1.8009999999999999</v>
+      </c>
       <c r="G54" s="3">
         <v>2121.8526321087065</v>
       </c>
@@ -3103,6 +3409,12 @@
       <c r="D55" s="4">
         <v>1.03</v>
       </c>
+      <c r="E55" s="13">
+        <v>28908.274203177654</v>
+      </c>
+      <c r="F55" s="4">
+        <v>4.0350000000000001</v>
+      </c>
       <c r="G55" s="3">
         <v>2092.9796918632642</v>
       </c>
@@ -3141,6 +3453,12 @@
       <c r="D56" s="4">
         <v>0.1535</v>
       </c>
+      <c r="E56" s="13">
+        <v>29314.69773399015</v>
+      </c>
+      <c r="F56" s="4">
+        <v>1.1547081085126265</v>
+      </c>
       <c r="G56" s="3">
         <v>1993.2258784893268</v>
       </c>
@@ -3179,8 +3497,12 @@
       <c r="D57" s="4">
         <v>0.58505732297668167</v>
       </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="E57" s="13">
+        <v>25880.852123076918</v>
+      </c>
+      <c r="F57" s="4">
+        <v>3.7949999999999999</v>
+      </c>
       <c r="G57" s="3">
         <v>2206.3749076923077</v>
       </c>
@@ -3219,8 +3541,12 @@
       <c r="D58" s="4">
         <v>1.0880000000000001</v>
       </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
+      <c r="E58" s="13">
+        <v>30109.662913143733</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0.68397241992440561</v>
+      </c>
       <c r="G58" s="3">
         <v>2410.7717778631823</v>
       </c>
@@ -3259,8 +3585,12 @@
       <c r="D59" s="4">
         <v>1.381</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="E59" s="13">
+        <v>27250.278787878789</v>
+      </c>
+      <c r="F59" s="4">
+        <v>4.3550000000000004</v>
+      </c>
       <c r="G59" s="3">
         <v>2063.065768799102</v>
       </c>
@@ -3299,8 +3629,12 @@
       <c r="D60" s="4">
         <v>0.96140000000000003</v>
       </c>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
+      <c r="E60" s="13">
+        <v>28527.905436787845</v>
+      </c>
+      <c r="F60" s="4">
+        <v>3.7639999999999998</v>
+      </c>
       <c r="G60" s="3">
         <v>2130.8304612045577</v>
       </c>
@@ -3339,8 +3673,12 @@
       <c r="D61" s="4">
         <v>1.0660000000000001</v>
       </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
+      <c r="E61" s="13">
+        <v>29057.637773437495</v>
+      </c>
+      <c r="F61" s="4">
+        <v>4.4779999999999998</v>
+      </c>
       <c r="G61" s="3">
         <v>2051.3616796874999</v>
       </c>
@@ -3379,8 +3717,12 @@
       <c r="D62" s="4">
         <v>1.0840000000000001</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="E62" s="13">
+        <v>28700.304673439769</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0.22692772181853582</v>
+      </c>
       <c r="G62" s="3">
         <v>1909.6693952588291</v>
       </c>
@@ -3419,8 +3761,12 @@
       <c r="D63" s="4">
         <v>1.2130000000000001</v>
       </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
+      <c r="E63" s="13">
+        <v>29603.535327635331</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0.73699606608904666</v>
+      </c>
       <c r="G63" s="3">
         <v>1945.571082621083</v>
       </c>
@@ -3459,8 +3805,12 @@
       <c r="D64" s="4">
         <v>0.5857</v>
       </c>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
+      <c r="E64" s="13">
+        <v>30796.591161548742</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.28736877061176075</v>
+      </c>
       <c r="G64" s="3">
         <v>1865.6304272363154</v>
       </c>
@@ -3499,8 +3849,12 @@
       <c r="D65" s="4">
         <v>0.96840000000000004</v>
       </c>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
+      <c r="E65" s="13">
+        <v>26433.200698896475</v>
+      </c>
+      <c r="F65" s="4">
+        <v>9.5922240269476433E-2</v>
+      </c>
       <c r="G65" s="3">
         <v>2093.699143457698</v>
       </c>
@@ -3539,8 +3893,12 @@
       <c r="D66" s="4">
         <v>0.67720000000000002</v>
       </c>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+      <c r="E66" s="13">
+        <v>28440.116411960134</v>
+      </c>
+      <c r="F66" s="4">
+        <v>1.7703704389059354</v>
+      </c>
       <c r="G66" s="3">
         <v>2026.2012244897958</v>
       </c>
@@ -3579,8 +3937,12 @@
       <c r="D67" s="4">
         <v>0.82140000000000002</v>
       </c>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
+      <c r="E67" s="13">
+        <v>28559.124155844151</v>
+      </c>
+      <c r="F67" s="4">
+        <v>3.7309999999999999</v>
+      </c>
       <c r="G67" s="3">
         <v>2290.8622597402596</v>
       </c>
@@ -3619,8 +3981,12 @@
       <c r="D68" s="4">
         <v>1.474</v>
       </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
+      <c r="E68" s="13">
+        <v>27660.979712437089</v>
+      </c>
+      <c r="F68" s="4">
+        <v>2.9660000000000002</v>
+      </c>
       <c r="G68" s="3">
         <v>2272.5285255212075</v>
       </c>
@@ -3659,8 +4025,12 @@
       <c r="D69" s="4">
         <v>1.2929999999999999</v>
       </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
+      <c r="E69" s="13">
+        <v>26887.473244781784</v>
+      </c>
+      <c r="F69" s="4">
+        <v>4.08</v>
+      </c>
       <c r="G69" s="3">
         <v>2175.474003795066</v>
       </c>
@@ -3699,8 +4069,12 @@
       <c r="D70" s="4">
         <v>0.81640000000000001</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+      <c r="E70" s="13">
+        <v>28811.381380337643</v>
+      </c>
+      <c r="F70" s="4">
+        <v>4.8449999999999998</v>
+      </c>
       <c r="G70" s="3">
         <v>1919.4449702085406</v>
       </c>
@@ -3739,8 +4113,12 @@
       <c r="D71" s="4">
         <v>0.74139999999999995</v>
       </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="E71" s="13">
+        <v>30867.519809193403</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.21837763470863425</v>
+      </c>
       <c r="G71" s="3">
         <v>2106.7701908065915</v>
       </c>
@@ -3779,8 +4157,12 @@
       <c r="D72" s="4">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
+      <c r="E72" s="13">
+        <v>28182.120419370938</v>
+      </c>
+      <c r="F72" s="4">
+        <v>4.391</v>
+      </c>
       <c r="G72" s="3">
         <v>2129.8228657014479</v>
       </c>
@@ -3819,8 +4201,12 @@
       <c r="D73" s="4">
         <v>0.65539999999999998</v>
       </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
+      <c r="E73" s="13">
+        <v>28473.972724137933</v>
+      </c>
+      <c r="F73" s="4">
+        <v>4.25</v>
+      </c>
       <c r="G73" s="3">
         <v>1882.6717758620691</v>
       </c>
@@ -3859,8 +4245,12 @@
       <c r="D74" s="4">
         <v>0.504</v>
       </c>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
+      <c r="E74" s="13">
+        <v>29176.869679168543</v>
+      </c>
+      <c r="F74" s="4">
+        <v>3.14</v>
+      </c>
       <c r="G74" s="3">
         <v>2004.5937867148666</v>
       </c>
@@ -3899,8 +4289,12 @@
       <c r="D75" s="4">
         <v>1.044</v>
       </c>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
+      <c r="E75" s="13">
+        <v>25484.902503801324</v>
+      </c>
+      <c r="F75" s="4">
+        <v>2.794</v>
+      </c>
       <c r="G75" s="3">
         <v>1897.3531474911306</v>
       </c>
@@ -3939,8 +4333,12 @@
       <c r="D76" s="4">
         <v>0.95660000000000001</v>
       </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
+      <c r="E76" s="13">
+        <v>25309.034020456333</v>
+      </c>
+      <c r="F76" s="4">
+        <v>2.52</v>
+      </c>
       <c r="G76" s="3">
         <v>1877.1903304484656</v>
       </c>
@@ -3979,8 +4377,12 @@
       <c r="D77" s="4">
         <v>1.4610000000000001</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
+      <c r="E77" s="13">
+        <v>28202.85908059702</v>
+      </c>
+      <c r="F77" s="4">
+        <v>3.0230000000000001</v>
+      </c>
       <c r="G77" s="8">
         <v>2144.4570268656721</v>
       </c>
@@ -4019,8 +4421,12 @@
       <c r="D78" s="4">
         <v>1.0029999999999999</v>
       </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
+      <c r="E78" s="13">
+        <v>27410.482902967127</v>
+      </c>
+      <c r="F78" s="4">
+        <v>2.536</v>
+      </c>
       <c r="G78" s="8">
         <v>2269.9390280673624</v>
       </c>
@@ -4059,8 +4465,12 @@
       <c r="D79" s="4">
         <v>0.73319999999999996</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
+      <c r="E79" s="13">
+        <v>26364.712033195028</v>
+      </c>
+      <c r="F79" s="4">
+        <v>3.0470000000000002</v>
+      </c>
       <c r="G79" s="8">
         <v>2142.5337759336103</v>
       </c>
@@ -4099,8 +4509,12 @@
       <c r="D80" s="4">
         <v>1.0960000000000001</v>
       </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
+      <c r="E80" s="13">
+        <v>26017.914238603302</v>
+      </c>
+      <c r="F80" s="4">
+        <v>2.7080000000000002</v>
+      </c>
       <c r="G80" s="8">
         <v>1950.8415130940837</v>
       </c>
@@ -4139,8 +4553,12 @@
       <c r="D81" s="4">
         <v>1.1879999999999999</v>
       </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
+      <c r="E81" s="13">
+        <v>26663.247386759584</v>
+      </c>
+      <c r="F81" s="4">
+        <v>3.09</v>
+      </c>
       <c r="G81" s="8">
         <v>1994.0029865604777</v>
       </c>
@@ -4179,8 +4597,12 @@
       <c r="D82" s="4">
         <v>1.0580000000000001</v>
       </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
+      <c r="E82" s="13">
+        <v>26010.291922569297</v>
+      </c>
+      <c r="F82" s="4">
+        <v>3.802</v>
+      </c>
       <c r="G82" s="8">
         <v>1991.5499032116147</v>
       </c>
@@ -4219,8 +4641,12 @@
       <c r="D83" s="4">
         <v>0.76829999999999998</v>
       </c>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
+      <c r="E83" s="13">
+        <v>29613.426673170728</v>
+      </c>
+      <c r="F83" s="4">
+        <v>2.5179999999999998</v>
+      </c>
       <c r="G83" s="8">
         <v>2021.6803951219511</v>
       </c>
@@ -4259,8 +4685,12 @@
       <c r="D84" s="4">
         <v>1.155</v>
       </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
+      <c r="E84" s="13">
+        <v>24877.433790044357</v>
+      </c>
+      <c r="F84" s="4">
+        <v>1.462</v>
+      </c>
       <c r="G84" s="8">
         <v>2349.0291572203059</v>
       </c>
@@ -4299,8 +4729,12 @@
       <c r="D85" s="4">
         <v>0.47499999999999998</v>
       </c>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
+      <c r="E85" s="13">
+        <v>28632.672219476022</v>
+      </c>
+      <c r="F85" s="4">
+        <v>3.3650000000000002</v>
+      </c>
       <c r="G85" s="8">
         <v>2071.5530004943148</v>
       </c>
@@ -4339,8 +4773,12 @@
       <c r="D86" s="4">
         <v>0.4037</v>
       </c>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
+      <c r="E86" s="13">
+        <v>27330.990516478112</v>
+      </c>
+      <c r="F86" s="4">
+        <v>1.974</v>
+      </c>
       <c r="G86" s="8">
         <v>2201.0589916379731</v>
       </c>
@@ -4379,8 +4817,12 @@
       <c r="D87" s="4">
         <v>0.44619999999999999</v>
       </c>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
+      <c r="E87" s="13">
+        <v>27917.491898734181</v>
+      </c>
+      <c r="F87" s="4">
+        <v>1.6830000000000001</v>
+      </c>
       <c r="G87" s="8">
         <v>2380.766930379747</v>
       </c>
@@ -4419,8 +4861,12 @@
       <c r="D88" s="4">
         <v>0.79510000000000003</v>
       </c>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
+      <c r="E88" s="13">
+        <v>26934.494175334326</v>
+      </c>
+      <c r="F88" s="4">
+        <v>2.4239999999999999</v>
+      </c>
       <c r="G88" s="8">
         <v>2431.0453261515609</v>
       </c>
@@ -4459,8 +4905,12 @@
       <c r="D89" s="4">
         <v>0.64529999999999998</v>
       </c>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
+      <c r="E89" s="13">
+        <v>23414.118171745155</v>
+      </c>
+      <c r="F89" s="4">
+        <v>2.0249999999999999</v>
+      </c>
       <c r="G89" s="8">
         <v>1857.5073407202217</v>
       </c>
@@ -4499,8 +4949,12 @@
       <c r="D90" s="4">
         <v>0.81469999999999998</v>
       </c>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
+      <c r="E90" s="13">
+        <v>26039.125798525798</v>
+      </c>
+      <c r="F90" s="4">
+        <v>2.39</v>
+      </c>
       <c r="G90" s="8">
         <v>2241.1202653562659</v>
       </c>
@@ -4539,8 +4993,12 @@
       <c r="D91" s="4">
         <v>0.97289999999999999</v>
       </c>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
+      <c r="E91" s="13">
+        <v>26010.641878816339</v>
+      </c>
+      <c r="F91" s="4">
+        <v>2.028</v>
+      </c>
       <c r="G91" s="8">
         <v>2087.1034664161571</v>
       </c>
@@ -4579,8 +5037,12 @@
       <c r="D92" s="4">
         <v>1.2330000000000001</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
+      <c r="E92" s="13">
+        <v>28240.359752498818</v>
+      </c>
+      <c r="F92" s="4">
+        <v>3.7959999999999998</v>
+      </c>
       <c r="G92" s="8">
         <v>2068.1524036173255</v>
       </c>
@@ -4619,8 +5081,12 @@
       <c r="D93" s="4">
         <v>1.405</v>
       </c>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
+      <c r="E93" s="13">
+        <v>28492.491493383746</v>
+      </c>
+      <c r="F93" s="4">
+        <v>3.0049999999999999</v>
+      </c>
       <c r="G93" s="8">
         <v>1879.2003780718337</v>
       </c>
@@ -4659,8 +5125,12 @@
       <c r="D94" s="4">
         <v>0.72419999999999995</v>
       </c>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
+      <c r="E94" s="13">
+        <v>27763.123297823066</v>
+      </c>
+      <c r="F94" s="4">
+        <v>3.7360000000000002</v>
+      </c>
       <c r="G94" s="8">
         <v>2181.2708476146368</v>
       </c>
@@ -4699,8 +5169,12 @@
       <c r="D95" s="4">
         <v>1.129</v>
       </c>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
+      <c r="E95" s="13">
+        <v>25203.447582417579</v>
+      </c>
+      <c r="F95" s="4">
+        <v>4.0720000000000001</v>
+      </c>
       <c r="G95" s="8">
         <v>2150.549175824176</v>
       </c>
@@ -4739,8 +5213,12 @@
       <c r="D96" s="4">
         <v>0.56159999999999999</v>
       </c>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
+      <c r="E96" s="13">
+        <v>25803.147653631288</v>
+      </c>
+      <c r="F96" s="4">
+        <v>1.6659999999999999</v>
+      </c>
       <c r="G96" s="8">
         <v>1961.1552234636874</v>
       </c>
@@ -4783,8 +5261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6057,13 +6535,13 @@
       <c r="D30" s="4">
         <v>1.272</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="11">
         <v>3445.2866761865039</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="12">
         <v>1.2330000000000001</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="11">
         <v>933.36459565422763</v>
       </c>
       <c r="H30" s="4">
@@ -6101,9 +6579,13 @@
       <c r="D31" s="4">
         <v>0.56630000000000003</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="3">
+      <c r="E31" s="11">
+        <v>5298.4106203259826</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1.9219999999999999</v>
+      </c>
+      <c r="G31" s="11">
         <v>1053.9154170661557</v>
       </c>
       <c r="H31" s="4">
@@ -6141,9 +6623,13 @@
       <c r="D32" s="4">
         <v>0.96799999999999997</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="3">
+      <c r="E32" s="11">
+        <v>4276.773839014375</v>
+      </c>
+      <c r="F32" s="12">
+        <v>2.613</v>
+      </c>
+      <c r="G32" s="11">
         <v>1046.6198821355235</v>
       </c>
       <c r="H32" s="4">
@@ -7123,10 +7609,10 @@
       <c r="J54" s="4">
         <v>1.77</v>
       </c>
-      <c r="K54" s="12">
+      <c r="K54" s="11">
         <v>3948.7445082153336</v>
       </c>
-      <c r="L54" s="13">
+      <c r="L54" s="12">
         <v>2.3010788473402046</v>
       </c>
       <c r="M54" s="3">
@@ -9279,8 +9765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9362,6 +9848,12 @@
       <c r="C3" s="4">
         <v>0.52410000000000001</v>
       </c>
+      <c r="D3" s="13">
+        <v>10405.245716242662</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3.9660000000000002</v>
+      </c>
       <c r="F3" s="3">
         <v>1119.8579187866928</v>
       </c>
@@ -9397,6 +9889,12 @@
       <c r="C4" s="4">
         <v>0.58640000000000003</v>
       </c>
+      <c r="D4" s="13">
+        <v>10703.978358881877</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.476</v>
+      </c>
       <c r="F4" s="3">
         <v>1128.2125338142473</v>
       </c>
@@ -9432,6 +9930,12 @@
       <c r="C5" s="4">
         <v>1.462</v>
       </c>
+      <c r="D5" s="13">
+        <v>10793.927575757574</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3.4260000000000002</v>
+      </c>
       <c r="F5" s="3">
         <v>1190.8405757575758</v>
       </c>
@@ -9467,6 +9971,12 @@
       <c r="C6" s="4">
         <v>0.82299999999999995</v>
       </c>
+      <c r="D6" s="13">
+        <v>11001.474988834299</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3.8029999999999999</v>
+      </c>
       <c r="F6" s="3">
         <v>1136.3301277355963</v>
       </c>
@@ -9502,6 +10012,12 @@
       <c r="C7" s="4">
         <v>1.456</v>
       </c>
+      <c r="D7" s="13">
+        <v>10766.68572522738</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4.4470000000000001</v>
+      </c>
       <c r="F7" s="3">
         <v>1118.5278989947342</v>
       </c>
@@ -9537,6 +10053,12 @@
       <c r="C8" s="4">
         <v>0.7802</v>
       </c>
+      <c r="D8" s="13">
+        <v>10705.434775280897</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.76144636251120734</v>
+      </c>
       <c r="F8" s="3">
         <v>1107.92254494382</v>
       </c>
@@ -9572,6 +10094,12 @@
       <c r="C9" s="4">
         <v>0.88870000000000005</v>
       </c>
+      <c r="D9" s="13">
+        <v>11186.887611744083</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.7534071530063973</v>
+      </c>
       <c r="F9" s="3">
         <v>1131.7616524978089</v>
       </c>
@@ -9607,6 +10135,12 @@
       <c r="C10" s="4">
         <v>1.466</v>
       </c>
+      <c r="D10" s="13">
+        <v>10996.836237350508</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.78</v>
+      </c>
       <c r="F10" s="3">
         <v>1122.332672953082</v>
       </c>
@@ -9642,6 +10176,12 @@
       <c r="C11" s="4">
         <v>1.1040000000000001</v>
       </c>
+      <c r="D11" s="13">
+        <v>11257.359351403678</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.786</v>
+      </c>
       <c r="F11" s="3">
         <v>1136.6126108422072</v>
       </c>
@@ -9676,6 +10216,12 @@
       </c>
       <c r="C12" s="4">
         <v>0.2702</v>
+      </c>
+      <c r="D12" s="13">
+        <v>10851.995344673234</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.1819999999999999</v>
       </c>
       <c r="F12" s="3">
         <v>1155.510442256043</v>

</xml_diff>